<commit_message>
[FIX] Various fixes: see packages docs
</commit_message>
<xml_diff>
--- a/z0bug_odoo/data/account_invoice.xlsx
+++ b/z0bug_odoo/data/account_invoice.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="78">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -94,7 +94,7 @@
     <t xml:space="preserve">P1/2021/0001</t>
   </si>
   <si>
-    <t xml:space="preserve">-62</t>
+    <t xml:space="preserve">-35</t>
   </si>
   <si>
     <t xml:space="preserve">z0bug.invoice_Z0_2</t>
@@ -187,7 +187,7 @@
     <t xml:space="preserve">21/TO/1234</t>
   </si>
   <si>
-    <t xml:space="preserve">-68</t>
+    <t xml:space="preserve">-39</t>
   </si>
   <si>
     <t xml:space="preserve">z0bug.invoice_ZI_3</t>
@@ -199,7 +199,7 @@
     <t xml:space="preserve">XE125432</t>
   </si>
   <si>
-    <t xml:space="preserve">-66</t>
+    <t xml:space="preserve">-38</t>
   </si>
   <si>
     <t xml:space="preserve">z0bug.invoice_ZI_4</t>
@@ -208,6 +208,9 @@
     <t xml:space="preserve">XE125439</t>
   </si>
   <si>
+    <t xml:space="preserve">-37</t>
+  </si>
+  <si>
     <t xml:space="preserve">z0bug.invoice_ZI_5</t>
   </si>
   <si>
@@ -217,6 +220,9 @@
     <t xml:space="preserve">FATT/0123/21</t>
   </si>
   <si>
+    <t xml:space="preserve">-36</t>
+  </si>
+  <si>
     <t xml:space="preserve">z0bug.invoice_ZI_6</t>
   </si>
   <si>
@@ -244,7 +250,7 @@
     <t xml:space="preserve">TI-8778</t>
   </si>
   <si>
-    <t xml:space="preserve">-70</t>
+    <t xml:space="preserve">-42</t>
   </si>
   <si>
     <t xml:space="preserve">z0bug.fiscalpos_xx</t>
@@ -365,7 +371,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F19" activeCellId="0" sqref="F19:G19"/>
+      <selection pane="bottomLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -796,8 +802,8 @@
       <c r="F13" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="G13" s="2" t="n">
-        <v>-62</v>
+      <c r="G13" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>50</v>
@@ -829,8 +835,8 @@
       <c r="F14" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="G14" s="2" t="n">
-        <v>-62</v>
+      <c r="G14" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>50</v>
@@ -859,11 +865,11 @@
       <c r="E15" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F15" s="2" t="n">
-        <v>-64</v>
-      </c>
-      <c r="G15" s="2" t="n">
-        <v>-62</v>
+      <c r="F15" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>50</v>
@@ -880,23 +886,23 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F16" s="2" t="n">
-        <v>-63</v>
-      </c>
-      <c r="G16" s="2" t="n">
-        <v>-62</v>
+        <v>65</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>50</v>
@@ -913,23 +919,23 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G17" s="2" t="n">
-        <v>-62</v>
+      <c r="G17" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>50</v>
@@ -938,7 +944,7 @@
         <v>51</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>19</v>
@@ -946,26 +952,26 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>53</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G18" s="2" t="n">
-        <v>-62</v>
+      <c r="G18" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>51</v>
@@ -979,20 +985,20 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>24</v>
@@ -1004,7 +1010,7 @@
         <v>51</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
[IMP] New features, mainly please + arcangelo
</commit_message>
<xml_diff>
--- a/z0bug_odoo/data/account_invoice.xlsx
+++ b/z0bug_odoo/data/account_invoice.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="119">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -362,6 +362,21 @@
   </si>
   <si>
     <t xml:space="preserve">DE/22/9876</t>
+  </si>
+  <si>
+    <t xml:space="preserve">z0bug.invoice_ZI_10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contract</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CH/22/0626</t>
+  </si>
+  <si>
+    <t xml:space="preserve">####-##-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">base.USD</t>
   </si>
 </sst>
 </file>
@@ -529,14 +544,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S21"/>
+  <dimension ref="A1:S1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="F21" activeCellId="0" sqref="F21"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A22" activeCellId="0" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1563,6 +1578,53 @@
         <v>1</v>
       </c>
     </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="K22" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="L22" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="M22" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="N22" s="4"/>
+      <c r="O22" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="S22" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>